<commit_message>
add place holder and description
</commit_message>
<xml_diff>
--- a/resources/l10n/app_en.xlsx
+++ b/resources/l10n/app_en.xlsx
@@ -24,32 +24,55 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>discover</t>
   </si>
   <si>
+    <t>profile</t>
+  </si>
+  <si>
     <t>Discover</t>
   </si>
   <si>
-    <t>profile</t>
-  </si>
-  <si>
     <t>Profile</t>
   </si>
   <si>
-    <t>Setting</t>
-  </si>
-  <si>
-    <t>setting</t>
+    <t>About Discover</t>
+  </si>
+  <si>
+    <t>About Profile</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Description(Optional)</t>
+  </si>
+  <si>
+    <t>Placeholder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name:String </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -77,8 +100,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -359,36 +383,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>